<commit_message>
First Draft of Creatures Excel
- First draft Creatures Excel complete
- Botched attempted to repair Vik´s Battle Simulation
</commit_message>
<xml_diff>
--- a/Game Design/Creatures.xlsx
+++ b/Game Design/Creatures.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
   <si>
     <t>Name Enemy</t>
   </si>
@@ -143,6 +143,51 @@
   </si>
   <si>
     <t>silver</t>
+  </si>
+  <si>
+    <t>double damage attack</t>
+  </si>
+  <si>
+    <t>debuffing attack</t>
+  </si>
+  <si>
+    <t>Poisoning attack ( extended damage)</t>
+  </si>
+  <si>
+    <t>freeze (paralizing attack)</t>
+  </si>
+  <si>
+    <t>doubedamage attack</t>
+  </si>
+  <si>
+    <t>basic</t>
+  </si>
+  <si>
+    <t>Posoning Trunk (dmg 3 rounds)</t>
+  </si>
+  <si>
+    <t>Eye for an Eye (reflects damage)</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>Trample (doubledamage)</t>
+  </si>
+  <si>
+    <t>healing wind (heal self)</t>
+  </si>
+  <si>
+    <t>Lion Pride (buff strength)</t>
+  </si>
+  <si>
+    <t>strength of the Jungle(armor buff)</t>
+  </si>
+  <si>
+    <t>Steal life (takes HP from player)</t>
+  </si>
+  <si>
+    <t>Curse (debuff)</t>
   </si>
 </sst>
 </file>
@@ -285,17 +330,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Berechnung" xfId="1" builtinId="22"/>
@@ -574,7 +648,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -585,12 +659,15 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="9"/>
+    <col min="11" max="11" width="39.5703125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -600,276 +677,468 @@
       <c r="B1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="9">
+      <c r="B2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="7">
         <v>1</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="D2" s="14">
+        <v>2</v>
+      </c>
+      <c r="E2" s="14">
+        <v>16</v>
+      </c>
+      <c r="F2" s="14">
+        <v>1</v>
+      </c>
+      <c r="G2" s="14">
+        <v>3</v>
+      </c>
+      <c r="H2" s="14">
+        <v>2</v>
+      </c>
+      <c r="I2" s="14">
+        <v>50</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="14">
+        <v>2</v>
+      </c>
+      <c r="E3" s="14">
+        <v>16</v>
+      </c>
+      <c r="F3" s="14">
+        <v>1</v>
+      </c>
+      <c r="G3" s="14">
+        <v>3</v>
+      </c>
+      <c r="H3" s="14">
+        <v>2</v>
+      </c>
+      <c r="I3" s="14">
+        <v>50</v>
+      </c>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="2">
+        <v>38</v>
+      </c>
+      <c r="C4" s="8">
         <v>1</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="D4" s="14">
+        <v>2</v>
+      </c>
+      <c r="E4" s="14">
+        <v>16</v>
+      </c>
+      <c r="F4" s="14">
+        <v>1</v>
+      </c>
+      <c r="G4" s="14">
+        <v>3</v>
+      </c>
+      <c r="H4" s="14">
+        <v>2</v>
+      </c>
+      <c r="I4" s="14">
+        <v>50</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14">
+        <v>2</v>
+      </c>
+      <c r="E5" s="14">
+        <v>16</v>
+      </c>
+      <c r="F5" s="14">
+        <v>1</v>
+      </c>
+      <c r="G5" s="14">
+        <v>3</v>
+      </c>
+      <c r="H5" s="14">
+        <v>2</v>
+      </c>
+      <c r="I5" s="14">
+        <v>50</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="8">
         <v>1</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="D6" s="14">
+        <v>2</v>
+      </c>
+      <c r="E6" s="14">
+        <v>16</v>
+      </c>
+      <c r="F6" s="14">
+        <v>1</v>
+      </c>
+      <c r="G6" s="14">
+        <v>3</v>
+      </c>
+      <c r="H6" s="14">
+        <v>2</v>
+      </c>
+      <c r="I6" s="14">
+        <v>50</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="2">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+      <c r="D7" s="14">
+        <v>2</v>
+      </c>
+      <c r="E7" s="14">
+        <v>16</v>
+      </c>
+      <c r="F7" s="14">
+        <v>1</v>
+      </c>
+      <c r="G7" s="14">
+        <v>3</v>
+      </c>
+      <c r="H7" s="14">
+        <v>2</v>
+      </c>
+      <c r="I7" s="14">
+        <v>50</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="K7" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="C8" s="8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="15">
+        <v>10</v>
+      </c>
+      <c r="E8" s="15">
+        <v>30</v>
+      </c>
+      <c r="F8" s="15">
+        <v>6</v>
+      </c>
+      <c r="G8" s="15">
+        <v>2</v>
+      </c>
+      <c r="H8" s="14">
+        <v>2</v>
+      </c>
+      <c r="I8" s="15">
+        <v>100</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="2">
-        <v>3</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2</v>
+      </c>
+      <c r="D9" s="15">
+        <v>10</v>
+      </c>
+      <c r="E9" s="15">
+        <v>30</v>
+      </c>
+      <c r="F9" s="15">
+        <v>6</v>
+      </c>
+      <c r="G9" s="15">
+        <v>2</v>
+      </c>
+      <c r="H9" s="14">
+        <v>2</v>
+      </c>
+      <c r="I9" s="15">
+        <v>100</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="C10" s="8">
+        <v>2</v>
+      </c>
+      <c r="D10" s="15">
+        <v>10</v>
+      </c>
+      <c r="E10" s="15">
+        <v>30</v>
+      </c>
+      <c r="F10" s="15">
+        <v>6</v>
+      </c>
+      <c r="G10" s="15">
+        <v>2</v>
+      </c>
+      <c r="H10" s="14">
+        <v>2</v>
+      </c>
+      <c r="I10" s="15">
+        <v>100</v>
+      </c>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2</v>
+      </c>
+      <c r="D11" s="15">
+        <v>10</v>
+      </c>
+      <c r="E11" s="15">
+        <v>30</v>
+      </c>
+      <c r="F11" s="15">
+        <v>6</v>
+      </c>
+      <c r="G11" s="15">
+        <v>2</v>
+      </c>
+      <c r="H11" s="14">
+        <v>2</v>
+      </c>
+      <c r="I11" s="15">
+        <v>100</v>
+      </c>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="2">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="C12" s="8">
+        <v>3</v>
+      </c>
+      <c r="D12" s="15">
+        <v>15</v>
+      </c>
+      <c r="E12" s="15">
+        <v>70</v>
+      </c>
+      <c r="F12" s="15">
+        <v>10</v>
+      </c>
+      <c r="G12" s="15">
+        <v>3</v>
+      </c>
+      <c r="H12" s="15">
+        <v>2</v>
+      </c>
+      <c r="I12" s="15">
+        <v>200</v>
+      </c>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="2">
-        <v>3</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="C13" s="8">
+        <v>3</v>
+      </c>
+      <c r="D13" s="15">
+        <v>15</v>
+      </c>
+      <c r="E13" s="15">
+        <v>70</v>
+      </c>
+      <c r="F13" s="15">
+        <v>10</v>
+      </c>
+      <c r="G13" s="15">
+        <v>3</v>
+      </c>
+      <c r="H13" s="15">
+        <v>2</v>
+      </c>
+      <c r="I13" s="15">
+        <v>200</v>
+      </c>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -878,38 +1147,70 @@
       <c r="B14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="2">
-        <v>3</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="C14" s="8">
+        <v>3</v>
+      </c>
+      <c r="D14" s="15">
+        <v>15</v>
+      </c>
+      <c r="E14" s="15">
+        <v>70</v>
+      </c>
+      <c r="F14" s="15">
+        <v>10</v>
+      </c>
+      <c r="G14" s="15">
+        <v>3</v>
+      </c>
+      <c r="H14" s="15">
+        <v>2</v>
+      </c>
+      <c r="I14" s="15">
+        <v>200</v>
+      </c>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L14" s="15" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="2">
-        <v>2</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="C15" s="8">
+        <v>3</v>
+      </c>
+      <c r="D15" s="15">
+        <v>15</v>
+      </c>
+      <c r="E15" s="15">
+        <v>70</v>
+      </c>
+      <c r="F15" s="15">
+        <v>10</v>
+      </c>
+      <c r="G15" s="15">
+        <v>3</v>
+      </c>
+      <c r="H15" s="15">
+        <v>2</v>
+      </c>
+      <c r="I15" s="15">
+        <v>200</v>
+      </c>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -918,30 +1219,42 @@
       <c r="B16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="2">
-        <v>3</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
+      <c r="C16" s="8">
+        <v>3</v>
+      </c>
+      <c r="D16" s="15">
+        <v>15</v>
+      </c>
+      <c r="E16" s="15">
+        <v>70</v>
+      </c>
+      <c r="F16" s="15">
+        <v>10</v>
+      </c>
+      <c r="G16" s="15">
+        <v>3</v>
+      </c>
+      <c r="H16" s="15">
+        <v>2</v>
+      </c>
+      <c r="I16" s="15">
+        <v>200</v>
+      </c>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16" s="15" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L16"/>
+  <autoFilter ref="A1:L16">
+    <sortState ref="A2:L16">
+      <sortCondition ref="C1:C16"/>
+    </sortState>
+  </autoFilter>
   <conditionalFormatting sqref="C2:C16">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -958,6 +1271,14 @@
         <color rgb="FF5A8AC6"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Creature Spawn and pictures
- Identified spawn tiles for each subcreature
-added pics for GDD
</commit_message>
<xml_diff>
--- a/Game Design/Creatures.xlsx
+++ b/Game Design/Creatures.xlsx
@@ -11,7 +11,7 @@
     <sheet name="OldList" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle2!$A$1:$M$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle2!$A$1:$M$15</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
   <si>
     <t>Name Enemy</t>
   </si>
@@ -130,21 +130,6 @@
     <t>Jackal</t>
   </si>
   <si>
-    <t>Basic</t>
-  </si>
-  <si>
-    <t>Ice</t>
-  </si>
-  <si>
-    <t>desert</t>
-  </si>
-  <si>
-    <t>jungle</t>
-  </si>
-  <si>
-    <t>silver</t>
-  </si>
-  <si>
     <t>double damage attack</t>
   </si>
   <si>
@@ -160,9 +145,6 @@
     <t>doubedamage attack</t>
   </si>
   <si>
-    <t>basic</t>
-  </si>
-  <si>
     <t>Posoning Trunk (dmg 3 rounds)</t>
   </si>
   <si>
@@ -187,10 +169,73 @@
     <t>Steal life (takes HP from player)</t>
   </si>
   <si>
-    <t>Curse (debuff)</t>
-  </si>
-  <si>
     <t>Primary Tile</t>
+  </si>
+  <si>
+    <t>GreenLion</t>
+  </si>
+  <si>
+    <t>Jungle</t>
+  </si>
+  <si>
+    <t>Arctic</t>
+  </si>
+  <si>
+    <t>HornedLion</t>
+  </si>
+  <si>
+    <t>Grassland&amp;Forest</t>
+  </si>
+  <si>
+    <t>Desert&amp;Savannah</t>
+  </si>
+  <si>
+    <t>SilverLion</t>
+  </si>
+  <si>
+    <t>Savannah</t>
+  </si>
+  <si>
+    <t>IceJackal</t>
+  </si>
+  <si>
+    <t>GreenJackal</t>
+  </si>
+  <si>
+    <t>DesertJackal</t>
+  </si>
+  <si>
+    <t>IceLion</t>
+  </si>
+  <si>
+    <t>DesertLion</t>
+  </si>
+  <si>
+    <t>SilverJackal</t>
+  </si>
+  <si>
+    <t>MammothParent</t>
+  </si>
+  <si>
+    <t>Grassland</t>
+  </si>
+  <si>
+    <t>GreenMammoth</t>
+  </si>
+  <si>
+    <t>IceMammoth</t>
+  </si>
+  <si>
+    <t>SilverMammoth</t>
+  </si>
+  <si>
+    <t>Forest (all)</t>
+  </si>
+  <si>
+    <t>DesertMammoth</t>
+  </si>
+  <si>
+    <t>Artic&amp;Forest</t>
   </si>
 </sst>
 </file>
@@ -372,7 +417,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -406,9 +451,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -692,7 +734,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -700,15 +742,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="8"/>
     <col min="12" max="12" width="39.5703125" style="8" customWidth="1"/>
     <col min="13" max="13" width="41.140625" customWidth="1"/>
@@ -716,8 +760,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>55</v>
+      <c r="A1" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>20</v>
@@ -757,21 +801,23 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="16" t="s">
-        <v>25</v>
+      <c r="A2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
       </c>
       <c r="E2" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="13">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -786,23 +832,25 @@
         <v>50</v>
       </c>
       <c r="K2" s="13">
-        <f t="shared" ref="K2:K17" si="0">F2*(E2+G2)</f>
-        <v>90</v>
+        <f>F2*(E2+G2)</f>
+        <v>140</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="17" t="s">
+      <c r="A3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D3" s="7">
         <v>1</v>
@@ -826,32 +874,34 @@
         <v>50</v>
       </c>
       <c r="K3" s="13">
-        <f t="shared" si="0"/>
+        <f>F3*(E3+G3)</f>
         <v>140</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="17" t="s">
+      <c r="A4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D4" s="7">
         <v>1</v>
       </c>
       <c r="E4" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" s="13">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G4" s="13">
         <v>1</v>
@@ -866,23 +916,25 @@
         <v>50</v>
       </c>
       <c r="K4" s="13">
-        <f t="shared" ref="K4" si="1">F4*(E4+G4)</f>
-        <v>140</v>
+        <f>F4*(E4+G4)</f>
+        <v>90</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="17" t="s">
-        <v>25</v>
+      <c r="A5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
@@ -906,195 +958,205 @@
         <v>50</v>
       </c>
       <c r="K5" s="13">
-        <f t="shared" si="0"/>
+        <f>F5*(E5+G5)</f>
         <v>140</v>
       </c>
       <c r="L5" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13">
+        <v>3</v>
+      </c>
+      <c r="F6" s="13">
+        <v>35</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>3</v>
+      </c>
+      <c r="I6" s="13">
+        <v>2</v>
+      </c>
+      <c r="J6" s="13">
+        <v>50</v>
+      </c>
+      <c r="K6" s="13">
+        <f>F6*(E6+G6)</f>
+        <v>140</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="14">
+        <v>5</v>
+      </c>
+      <c r="F7" s="14">
+        <v>70</v>
+      </c>
+      <c r="G7" s="14">
+        <v>3</v>
+      </c>
+      <c r="H7" s="13">
+        <v>3</v>
+      </c>
+      <c r="I7" s="13">
+        <v>2</v>
+      </c>
+      <c r="J7" s="14">
+        <v>100</v>
+      </c>
+      <c r="K7" s="13">
+        <f>F7*(E7+G7)</f>
+        <v>560</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="7">
+        <v>2</v>
+      </c>
+      <c r="E8" s="14">
+        <v>5</v>
+      </c>
+      <c r="F8" s="14">
+        <v>70</v>
+      </c>
+      <c r="G8" s="14">
+        <v>3</v>
+      </c>
+      <c r="H8" s="13">
+        <v>3</v>
+      </c>
+      <c r="I8" s="13">
+        <v>2</v>
+      </c>
+      <c r="J8" s="14">
+        <v>100</v>
+      </c>
+      <c r="K8" s="13">
+        <f>F8*(E8+G8)</f>
+        <v>560</v>
+      </c>
+      <c r="L8" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="7">
-        <v>2</v>
-      </c>
-      <c r="E6" s="13">
+      <c r="M8" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="7">
+        <v>2</v>
+      </c>
+      <c r="E9" s="14">
         <v>5</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F9" s="14">
         <v>70</v>
       </c>
-      <c r="G6" s="13">
-        <v>3</v>
-      </c>
-      <c r="H6" s="13">
-        <v>3</v>
-      </c>
-      <c r="I6" s="13">
-        <v>2</v>
-      </c>
-      <c r="J6" s="13">
+      <c r="G9" s="14">
+        <v>3</v>
+      </c>
+      <c r="H9" s="13">
+        <v>3</v>
+      </c>
+      <c r="I9" s="13">
+        <v>2</v>
+      </c>
+      <c r="J9" s="14">
         <v>100</v>
       </c>
-      <c r="K6" s="13">
-        <f t="shared" si="0"/>
+      <c r="K9" s="13">
+        <f>F9*(E9+G9)</f>
         <v>560</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="L9" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="M6" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="M9" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="7">
-        <v>3</v>
-      </c>
-      <c r="E7" s="13">
-        <v>10</v>
-      </c>
-      <c r="F7" s="13">
-        <v>100</v>
-      </c>
-      <c r="G7" s="13">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="7">
+        <v>2</v>
+      </c>
+      <c r="E10" s="13">
         <v>5</v>
       </c>
-      <c r="H7" s="13">
-        <v>3</v>
-      </c>
-      <c r="I7" s="13">
-        <v>2</v>
-      </c>
-      <c r="J7" s="13">
-        <v>200</v>
-      </c>
-      <c r="K7" s="13">
-        <f t="shared" si="0"/>
-        <v>1500</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="7">
-        <v>1</v>
-      </c>
-      <c r="E8" s="13">
-        <v>3</v>
-      </c>
-      <c r="F8" s="13">
-        <v>35</v>
-      </c>
-      <c r="G8" s="13">
-        <v>1</v>
-      </c>
-      <c r="H8" s="13">
-        <v>3</v>
-      </c>
-      <c r="I8" s="13">
-        <v>2</v>
-      </c>
-      <c r="J8" s="13">
-        <v>50</v>
-      </c>
-      <c r="K8" s="13">
-        <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="L8" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="7">
-        <v>1</v>
-      </c>
-      <c r="E9" s="14">
-        <v>3</v>
-      </c>
-      <c r="F9" s="14">
-        <v>35</v>
-      </c>
-      <c r="G9" s="14">
-        <v>1</v>
-      </c>
-      <c r="H9" s="13">
-        <v>3</v>
-      </c>
-      <c r="I9" s="13">
-        <v>2</v>
-      </c>
-      <c r="J9" s="14">
-        <v>50</v>
-      </c>
-      <c r="K9" s="13">
-        <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="7">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14">
-        <v>3</v>
-      </c>
-      <c r="F10" s="14">
-        <v>35</v>
-      </c>
-      <c r="G10" s="14">
-        <v>1</v>
+      <c r="F10" s="13">
+        <v>70</v>
+      </c>
+      <c r="G10" s="13">
+        <v>3</v>
       </c>
       <c r="H10" s="13">
         <v>3</v>
@@ -1106,63 +1168,67 @@
         <v>50</v>
       </c>
       <c r="K10" s="13">
-        <f t="shared" si="0"/>
-        <v>140</v>
+        <f>F10*(E10+G10)</f>
+        <v>560</v>
       </c>
       <c r="L10" s="14" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="17" t="s">
-        <v>34</v>
+      <c r="A11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="D11" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" s="14">
+        <v>10</v>
+      </c>
+      <c r="F11" s="14">
+        <v>100</v>
+      </c>
+      <c r="G11" s="14">
         <v>5</v>
       </c>
-      <c r="F11" s="14">
-        <v>70</v>
-      </c>
-      <c r="G11" s="14">
-        <v>3</v>
-      </c>
       <c r="H11" s="13">
         <v>3</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="14">
         <v>2</v>
       </c>
       <c r="J11" s="14">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="K11" s="13">
-        <f t="shared" si="0"/>
-        <v>560</v>
+        <f>F11*(E11+G11)</f>
+        <v>1500</v>
       </c>
       <c r="L11" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="17" t="s">
-        <v>34</v>
+      <c r="A12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="D12" s="7">
         <v>3</v>
@@ -1179,43 +1245,45 @@
       <c r="H12" s="13">
         <v>3</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="14">
         <v>2</v>
       </c>
       <c r="J12" s="14">
         <v>200</v>
       </c>
       <c r="K12" s="13">
-        <f t="shared" si="0"/>
+        <f>F12*(E12+G12)</f>
         <v>1500</v>
       </c>
       <c r="L12" s="14" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="M12" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="17" t="s">
-        <v>26</v>
+      <c r="B13" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="D13" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" s="14">
+        <v>10</v>
+      </c>
+      <c r="F13" s="14">
+        <v>100</v>
+      </c>
+      <c r="G13" s="14">
         <v>5</v>
       </c>
-      <c r="F13" s="14">
-        <v>70</v>
-      </c>
-      <c r="G13" s="14">
-        <v>3</v>
-      </c>
       <c r="H13" s="13">
         <v>3</v>
       </c>
@@ -1223,66 +1291,70 @@
         <v>2</v>
       </c>
       <c r="J13" s="14">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="K13" s="13">
-        <f t="shared" si="0"/>
-        <v>560</v>
+        <f>F13*(E13+G13)</f>
+        <v>1500</v>
       </c>
       <c r="L13" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M13" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="17" t="s">
+      <c r="A14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="7">
+        <v>3</v>
+      </c>
+      <c r="E14" s="14">
+        <v>10</v>
+      </c>
+      <c r="F14" s="14">
+        <v>100</v>
+      </c>
+      <c r="G14" s="14">
+        <v>5</v>
+      </c>
+      <c r="H14" s="13">
+        <v>3</v>
+      </c>
+      <c r="I14" s="14">
+        <v>2</v>
+      </c>
+      <c r="J14" s="14">
+        <v>200</v>
+      </c>
+      <c r="K14" s="13">
+        <f>F14*(E14+G14)</f>
+        <v>1500</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="7">
-        <v>2</v>
-      </c>
-      <c r="E14" s="14">
-        <v>5</v>
-      </c>
-      <c r="F14" s="14">
-        <v>70</v>
-      </c>
-      <c r="G14" s="14">
-        <v>3</v>
-      </c>
-      <c r="H14" s="13">
-        <v>3</v>
-      </c>
-      <c r="I14" s="14">
-        <v>2</v>
-      </c>
-      <c r="J14" s="14">
-        <v>100</v>
-      </c>
-      <c r="K14" s="13">
-        <f t="shared" si="0"/>
-        <v>560</v>
-      </c>
-      <c r="L14" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="M14" s="14" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="17" t="s">
-        <v>26</v>
+      <c r="A15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D15" s="7">
         <v>3</v>
@@ -1306,100 +1378,24 @@
         <v>200</v>
       </c>
       <c r="K15" s="13">
-        <f t="shared" si="0"/>
+        <f>F15*(E15+G15)</f>
         <v>1500</v>
       </c>
       <c r="L15" s="14" t="s">
         <v>41</v>
       </c>
       <c r="M15" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="7">
-        <v>3</v>
-      </c>
-      <c r="E16" s="14">
-        <v>10</v>
-      </c>
-      <c r="F16" s="14">
-        <v>100</v>
-      </c>
-      <c r="G16" s="14">
-        <v>5</v>
-      </c>
-      <c r="H16" s="13">
-        <v>3</v>
-      </c>
-      <c r="I16" s="14">
-        <v>2</v>
-      </c>
-      <c r="J16" s="14">
-        <v>200</v>
-      </c>
-      <c r="K16" s="13">
-        <f t="shared" si="0"/>
-        <v>1500</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="M16" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="7">
-        <v>3</v>
-      </c>
-      <c r="E17" s="14">
-        <v>10</v>
-      </c>
-      <c r="F17" s="14">
-        <v>100</v>
-      </c>
-      <c r="G17" s="14">
-        <v>5</v>
-      </c>
-      <c r="H17" s="13">
-        <v>3</v>
-      </c>
-      <c r="I17" s="14">
-        <v>2</v>
-      </c>
-      <c r="J17" s="14">
-        <v>200</v>
-      </c>
-      <c r="K17" s="13">
-        <f t="shared" si="0"/>
-        <v>1500</v>
-      </c>
-      <c r="L17" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="M17" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M17"/>
-  <conditionalFormatting sqref="D2:D17">
-    <cfRule type="colorScale" priority="5">
+  <autoFilter ref="A1:M15">
+    <sortState ref="A2:M15">
+      <sortCondition ref="D1:D15"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="D2:D15">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1407,7 +1403,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1417,7 +1413,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1431,7 +1427,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="6" id="{BD974CD7-AFE7-4B3F-A550-14DD0621E763}">
+          <x14:cfRule type="iconSet" priority="23" id="{BD974CD7-AFE7-4B3F-A550-14DD0621E763}">
             <x14:iconSet iconSet="3Stars">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1444,7 +1440,7 @@
               </x14:cfvo>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>D2:D17</xm:sqref>
+          <xm:sqref>D2:D15</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>